<commit_message>
grid view with template done
</commit_message>
<xml_diff>
--- a/media/grid_files/paygrid1.xlsx
+++ b/media/grid_files/paygrid1.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t xml:space="preserve">company</t>
   </si>
   <si>
-    <t xml:space="preserve">product</t>
+    <t xml:space="preserve">fsdgsdgdsgh</t>
   </si>
   <si>
     <t xml:space="preserve">vehical_type</t>
@@ -58,28 +58,22 @@
     <t xml:space="preserve">hdfc</t>
   </si>
   <si>
+    <t xml:space="preserve">Third Party</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gujarta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJ06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Motor Insurance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scooters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bike 150 CC To 600 CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Third Party</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gujarta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GJ06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc</t>
   </si>
   <si>
     <t xml:space="preserve">Two Wheeler Liability Policy</t>
@@ -417,12 +411,12 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.17"/>
   </cols>
@@ -466,32 +460,32 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="n">
         <f aca="false">I2*90/100</f>
@@ -503,31 +497,31 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="n">
         <f aca="false">I3*90/100</f>
@@ -539,31 +533,31 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1" t="n">
         <f aca="false">I4*90/100</f>
@@ -572,34 +566,34 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>15.5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K5" s="1" t="n">
         <f aca="false">I5*90/100</f>
@@ -608,34 +602,34 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K6" s="1" t="n">
         <f aca="false">I6*90/100</f>
@@ -644,34 +638,34 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="n">
         <f aca="false">I7*90/100</f>
@@ -680,34 +674,34 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K8" s="1" t="n">
         <f aca="false">I8*90/100</f>

</xml_diff>